<commit_message>
further dev in BOM and schematics
</commit_message>
<xml_diff>
--- a/V2/BOM.xlsx
+++ b/V2/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -46,13 +46,10 @@
     <t xml:space="preserve">PCB</t>
   </si>
   <si>
-    <t xml:space="preserve">5*3.5</t>
-  </si>
-  <si>
     <t xml:space="preserve">STC8H8K64U DIP40</t>
   </si>
   <si>
-    <t xml:space="preserve">IC Socket DIP 28</t>
+    <t xml:space="preserve">IC Socket DIP 40</t>
   </si>
   <si>
     <t xml:space="preserve">Pin Header 1x3</t>
@@ -67,12 +64,21 @@
     <t xml:space="preserve">Resistors</t>
   </si>
   <si>
+    <t xml:space="preserve">tmc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Capacitors</t>
   </si>
   <si>
+    <t xml:space="preserve">one encoder</t>
+  </si>
+  <si>
     <t xml:space="preserve">Diode</t>
   </si>
   <si>
+    <t xml:space="preserve">old mcu</t>
+  </si>
+  <si>
     <t xml:space="preserve">JST 2P Female</t>
   </si>
   <si>
@@ -91,6 +97,9 @@
     <t xml:space="preserve">JST 5P Male</t>
   </si>
   <si>
+    <t xml:space="preserve">Terminal Connectors</t>
+  </si>
+  <si>
     <t xml:space="preserve">Switch</t>
   </si>
   <si>
@@ -106,10 +115,25 @@
     <t xml:space="preserve">TMC2209</t>
   </si>
   <si>
-    <t xml:space="preserve">Display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Display Mounts</t>
+    <t xml:space="preserve">Pin Header </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDC 20P Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDC 20P Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ribbon 20P </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCD 12864B (ST7920)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spacer Male-Female 8mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Components</t>
   </si>
   <si>
     <t xml:space="preserve">**</t>
@@ -118,13 +142,31 @@
     <t xml:space="preserve">Delivery Fees</t>
   </si>
   <si>
+    <t xml:space="preserve">tmc2209</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Design, Testing and Manufacturing</t>
   </si>
   <si>
+    <t xml:space="preserve">encoder</t>
+  </si>
+  <si>
     <t xml:space="preserve">TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery micro ohm instant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery micro ohm 2-3 D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery RAM</t>
   </si>
 </sst>
 </file>
@@ -550,10 +592,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -563,9 +605,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="10.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="10.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -598,17 +641,17 @@
       <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="8" t="n">
+        <v>140</v>
+      </c>
       <c r="D2" s="9" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="10" t="n">
         <f aca="false">C2*D2</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>8</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F2" s="11"/>
       <c r="G2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -616,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="14" t="n">
         <v>160</v>
@@ -636,17 +679,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="14" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="15" t="n">
         <f aca="false">C4*D4</f>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
@@ -656,7 +699,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="14" t="n">
         <v>3</v>
@@ -676,7 +719,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="14" t="n">
         <v>3</v>
@@ -696,7 +739,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="14" t="n">
         <v>45</v>
@@ -716,18 +759,26 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6" t="n">
+        <v>5</v>
+      </c>
       <c r="E8" s="15" t="n">
         <f aca="false">C8*D8</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
+      <c r="I8" s="1" t="n">
+        <v>-290</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
@@ -739,20 +790,28 @@
       <c r="C9" s="14" t="n">
         <v>2.5</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="6" t="n">
+        <v>3</v>
+      </c>
       <c r="E9" s="15" t="n">
         <f aca="false">C9*D9</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="17"/>
+      <c r="I9" s="1" t="n">
+        <v>-60</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="14" t="n">
         <v>1</v>
@@ -766,23 +825,29 @@
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="17"/>
+      <c r="I10" s="1" t="n">
+        <v>-90</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C11" s="14" t="n">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D11" s="6" t="n">
         <v>4</v>
       </c>
       <c r="E11" s="15" t="n">
         <f aca="false">C11*D11</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="17"/>
@@ -792,17 +857,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12" s="14" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D12" s="6" t="n">
         <v>4</v>
       </c>
       <c r="E12" s="15" t="n">
         <f aca="false">C12*D12</f>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="17"/>
@@ -812,17 +877,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C13" s="14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="15" t="n">
         <f aca="false">C13*D13</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="17"/>
@@ -832,17 +897,17 @@
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C14" s="14" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D14" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="15" t="n">
         <f aca="false">C14*D14</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="17"/>
@@ -852,17 +917,17 @@
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C15" s="14" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="D15" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E15" s="15" t="n">
         <f aca="false">C15*D15</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="17"/>
@@ -872,17 +937,17 @@
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D16" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E16" s="15" t="n">
         <f aca="false">C16*D16</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="17"/>
@@ -892,15 +957,17 @@
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="C17" s="14" t="n">
+        <v>1</v>
+      </c>
       <c r="D17" s="6" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E17" s="15" t="n">
         <f aca="false">C17*D17</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="17"/>
@@ -910,15 +977,17 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="14"/>
+        <v>26</v>
+      </c>
+      <c r="C18" s="14" t="n">
+        <v>8</v>
+      </c>
       <c r="D18" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E18" s="15" t="n">
         <f aca="false">C18*D18</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F18" s="16"/>
       <c r="G18" s="17"/>
@@ -928,17 +997,17 @@
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19" s="14" t="n">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="D19" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E19" s="15" t="n">
         <f aca="false">C19*D19</f>
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
@@ -948,37 +1017,37 @@
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C20" s="14" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="D20" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E20" s="15" t="n">
         <f aca="false">C20*D20</f>
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="F20" s="16"/>
-      <c r="G20" s="18"/>
+      <c r="G20" s="17"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C21" s="14" t="n">
-        <v>290</v>
+        <v>3</v>
       </c>
       <c r="D21" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="15" t="n">
         <f aca="false">C21*D21</f>
-        <v>290</v>
+        <v>6</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="18"/>
@@ -988,13 +1057,18 @@
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="14"/>
+        <v>30</v>
+      </c>
+      <c r="C22" s="14" t="n">
+        <v>290</v>
+      </c>
       <c r="D22" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="15"/>
+      <c r="E22" s="15" t="n">
+        <f aca="false">C22*D22</f>
+        <v>290</v>
+      </c>
       <c r="F22" s="16"/>
       <c r="G22" s="18"/>
     </row>
@@ -1003,95 +1077,257 @@
         <v>22</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="15"/>
+        <v>31</v>
+      </c>
+      <c r="C23" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="D23" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="15" t="n">
+        <f aca="false">C23*D23</f>
+        <v>4</v>
+      </c>
       <c r="F23" s="16"/>
       <c r="G23" s="18"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="15"/>
+      <c r="A24" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="D24" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="15" t="n">
+        <f aca="false">C24*D24</f>
+        <v>5</v>
+      </c>
       <c r="F24" s="16"/>
       <c r="G24" s="18"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
-        <v>30</v>
+      <c r="A25" s="6" t="n">
+        <v>24</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="C25" s="14" t="n">
+        <v>6</v>
+      </c>
       <c r="D25" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E25" s="15" t="n">
         <f aca="false">C25*D25</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F25" s="16"/>
-      <c r="G25" s="17"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="15"/>
-      <c r="G26" s="17"/>
+      <c r="A26" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D26" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="15" t="n">
+        <f aca="false">C26*D26</f>
+        <v>10</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" s="22" t="n">
+      <c r="A27" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="14" t="n">
+        <v>520</v>
+      </c>
+      <c r="D27" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="15" t="n">
         <f aca="false">C27*D27</f>
-        <v>0</v>
+        <v>520</v>
       </c>
       <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26"/>
+      <c r="A28" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="D28" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E28" s="15" t="n">
+        <f aca="false">C28*D28</f>
+        <v>16</v>
+      </c>
       <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2"/>
-      <c r="B29" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="3" t="n">
+      <c r="A29" s="6"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="1" t="n">
         <f aca="false">SUM(E2:E28)</f>
-        <v>706.5</v>
-      </c>
-      <c r="F29" s="30"/>
-      <c r="G29" s="31"/>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>1480.5</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="14" t="n">
+        <v>80</v>
+      </c>
+      <c r="D30" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" s="15" t="n">
+        <f aca="false">C30*D30</f>
+        <v>160</v>
+      </c>
+      <c r="F30" s="16"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="15"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="21" t="n">
+        <v>800</v>
+      </c>
+      <c r="D32" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="22" t="n">
+        <f aca="false">C32*D32</f>
+        <v>800</v>
+      </c>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2"/>
+      <c r="B34" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="28"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="3" t="n">
+        <f aca="false">SUM(E2:E33)</f>
+        <v>2440.5</v>
+      </c>
+      <c r="F34" s="30"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <f aca="false">I29-I30-I31-I32</f>
+        <v>1040.5</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
added control mode switch
</commit_message>
<xml_diff>
--- a/V2/BOM.xlsx
+++ b/V2/BOM.xlsx
@@ -594,8 +594,8 @@
   </sheetPr>
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -843,11 +843,11 @@
         <v>1</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E11" s="15" t="n">
         <f aca="false">C11*D11</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="17"/>
@@ -863,11 +863,11 @@
         <v>8</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" s="15" t="n">
         <f aca="false">C12*D12</f>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="17"/>
@@ -983,11 +983,11 @@
         <v>8</v>
       </c>
       <c r="D18" s="6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="15" t="n">
         <f aca="false">C18*D18</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F18" s="16"/>
       <c r="G18" s="17"/>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="I29" s="1" t="n">
         <f aca="false">SUM(E2:E28)</f>
-        <v>1480.5</v>
+        <v>1497.5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,7 +1292,7 @@
       <c r="D34" s="29"/>
       <c r="E34" s="3" t="n">
         <f aca="false">SUM(E2:E33)</f>
-        <v>2440.5</v>
+        <v>2457.5</v>
       </c>
       <c r="F34" s="30"/>
       <c r="G34" s="31"/>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="I34" s="1" t="n">
         <f aca="false">I29-I30-I31-I32</f>
-        <v>1040.5</v>
+        <v>1057.5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
upgraded board to use l7805 instead of lm317
</commit_message>
<xml_diff>
--- a/V2/BOM.xlsx
+++ b/V2/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -46,10 +46,10 @@
     <t xml:space="preserve">PCB</t>
   </si>
   <si>
-    <t xml:space="preserve">STC8H8K64U DIP40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC Socket DIP 40</t>
+    <t xml:space="preserve">STC8H8K64U DIP28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC Socket DIP 28</t>
   </si>
   <si>
     <t xml:space="preserve">Pin Header 1x3</t>
@@ -58,27 +58,18 @@
     <t xml:space="preserve">Terminal 2Pin</t>
   </si>
   <si>
-    <t xml:space="preserve">LM338</t>
+    <t xml:space="preserve">L7805</t>
   </si>
   <si>
     <t xml:space="preserve">Resistors</t>
   </si>
   <si>
-    <t xml:space="preserve">tmc</t>
-  </si>
-  <si>
     <t xml:space="preserve">Capacitors</t>
   </si>
   <si>
-    <t xml:space="preserve">one encoder</t>
-  </si>
-  <si>
     <t xml:space="preserve">Diode</t>
   </si>
   <si>
-    <t xml:space="preserve">old mcu</t>
-  </si>
-  <si>
     <t xml:space="preserve">JST 2P Female</t>
   </si>
   <si>
@@ -133,40 +124,19 @@
     <t xml:space="preserve">Spacer Male-Female 8mm</t>
   </si>
   <si>
-    <t xml:space="preserve">Total Components</t>
-  </si>
-  <si>
     <t xml:space="preserve">**</t>
   </si>
   <si>
     <t xml:space="preserve">Delivery Fees</t>
   </si>
   <si>
-    <t xml:space="preserve">tmc2209</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Design, Testing and Manufacturing</t>
   </si>
   <si>
-    <t xml:space="preserve">encoder</t>
-  </si>
-  <si>
     <t xml:space="preserve">TOTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actual component</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delivery micro ohm instant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delivery micro ohm 2-3 D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delivery RAM</t>
   </si>
 </sst>
 </file>
@@ -177,7 +147,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -201,16 +171,23 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Aptos Narrow"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Aptos Narrow"/>
       <family val="0"/>
       <charset val="1"/>
@@ -225,8 +202,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF1C1C1C"/>
+        <bgColor rgb="FF333300"/>
       </patternFill>
     </fill>
   </fills>
@@ -446,132 +423,116 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -584,6 +545,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF1C1C1C"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -592,10 +613,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -642,14 +663,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="8" t="n">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="D2" s="9" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="10" t="n">
         <f aca="false">C2*D2</f>
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="12"/>
@@ -662,14 +683,14 @@
         <v>8</v>
       </c>
       <c r="C3" s="14" t="n">
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="D3" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="15" t="n">
         <f aca="false">C3*D3</f>
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="17"/>
@@ -742,14 +763,14 @@
         <v>12</v>
       </c>
       <c r="C7" s="14" t="n">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="D7" s="6" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="15" t="n">
         <f aca="false">C7*D7</f>
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="17"/>
@@ -762,30 +783,24 @@
         <v>13</v>
       </c>
       <c r="C8" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="6" t="n">
         <v>5</v>
       </c>
       <c r="E8" s="15" t="n">
         <f aca="false">C8*D8</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
-      <c r="I8" s="1" t="n">
-        <v>-290</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="14" t="n">
         <v>2.5</v>
@@ -799,19 +814,13 @@
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="17"/>
-      <c r="I9" s="1" t="n">
-        <v>-60</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="14" t="n">
         <v>1</v>
@@ -825,19 +834,13 @@
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="17"/>
-      <c r="I10" s="1" t="n">
-        <v>-90</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C11" s="14" t="n">
         <v>1</v>
@@ -857,7 +860,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" s="14" t="n">
         <v>8</v>
@@ -877,7 +880,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13" s="14" t="n">
         <v>2</v>
@@ -897,7 +900,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" s="14" t="n">
         <v>12</v>
@@ -917,7 +920,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C15" s="14" t="n">
         <v>3</v>
@@ -937,7 +940,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C16" s="14" t="n">
         <v>15</v>
@@ -957,7 +960,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C17" s="14" t="n">
         <v>1</v>
@@ -977,7 +980,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18" s="14" t="n">
         <v>8</v>
@@ -997,7 +1000,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C19" s="14" t="n">
         <v>11</v>
@@ -1017,7 +1020,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C20" s="14" t="n">
         <v>60</v>
@@ -1037,7 +1040,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C21" s="14" t="n">
         <v>3</v>
@@ -1057,7 +1060,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C22" s="14" t="n">
         <v>290</v>
@@ -1077,7 +1080,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C23" s="14" t="n">
         <v>4</v>
@@ -1097,7 +1100,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C24" s="14" t="n">
         <v>5</v>
@@ -1117,7 +1120,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C25" s="14" t="n">
         <v>6</v>
@@ -1137,7 +1140,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C26" s="14" t="n">
         <v>10</v>
@@ -1157,7 +1160,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C27" s="14" t="n">
         <v>520</v>
@@ -1177,7 +1180,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C28" s="14" t="n">
         <v>4</v>
@@ -1200,39 +1203,26 @@
       <c r="E29" s="15"/>
       <c r="F29" s="16"/>
       <c r="G29" s="18"/>
-      <c r="H29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I29" s="1" t="n">
-        <f aca="false">SUM(E2:E28)</f>
-        <v>1497.5</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C30" s="14" t="n">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="D30" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E30" s="15" t="n">
         <f aca="false">C30*D30</f>
-        <v>160</v>
+        <v>360</v>
       </c>
       <c r="F30" s="16"/>
       <c r="G30" s="17"/>
-      <c r="H30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" s="1" t="n">
-        <v>90</v>
-      </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6"/>
@@ -1241,92 +1231,49 @@
       <c r="D31" s="6"/>
       <c r="E31" s="15"/>
       <c r="G31" s="17"/>
-      <c r="H31" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I31" s="1" t="n">
-        <v>290</v>
-      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="21" t="n">
-        <v>800</v>
-      </c>
-      <c r="D32" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E32" s="22" t="n">
+      <c r="A32" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="15" t="n">
         <f aca="false">C32*D32</f>
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F32" s="16"/>
       <c r="G32" s="17"/>
-      <c r="H32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I32" s="1" t="n">
-        <v>60</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="26"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="22"/>
       <c r="F33" s="16"/>
       <c r="G33" s="17"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
-      <c r="B34" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="29"/>
+      <c r="B34" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="24"/>
+      <c r="D34" s="25"/>
       <c r="E34" s="3" t="n">
         <f aca="false">SUM(E2:E33)</f>
-        <v>2457.5</v>
-      </c>
-      <c r="F34" s="30"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I34" s="1" t="n">
-        <f aca="false">I29-I30-I31-I32</f>
-        <v>1057.5</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H36" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I36" s="1" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H37" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I37" s="1" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I38" s="1" t="n">
-        <v>130</v>
-      </c>
+        <v>1732.5</v>
+      </c>
+      <c r="F34" s="26"/>
+      <c r="G34" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>